<commit_message>
Treat geologic age as multi-valued field in exports
</commit_message>
<xml_diff>
--- a/geosamples-ingest-service/src/test/resources/test-export.xlsx
+++ b/geosamples-ingest-service/src/test/resources/test-export.xlsx
@@ -1,18 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <workbookPr date1904="false"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paytoncain/Documents/projects/geology/geosamples-ingest/geosamples-ingest-service/src/test/resources/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1783F56D-A326-FD42-8E13-CA65A115B3ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView xWindow="-50000" yWindow="500" windowWidth="50000" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Data Output" r:id="rId3" sheetId="1"/>
+    <sheet name="Data Output" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="102">
   <si>
     <t>GEOMAR</t>
   </si>
@@ -315,20 +323,27 @@
   </si>
   <si>
     <t>Other Component Code (6)</t>
+  </si>
+  <si>
+    <t>00</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -336,7 +351,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="darkGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
@@ -351,21 +366,334 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AQ6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AR6"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="true"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>58</v>
       </c>
@@ -495,8 +823,11 @@
       <c r="AQ1" t="s">
         <v>100</v>
       </c>
+      <c r="AR1" t="s">
+        <v>80</v>
+      </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -515,23 +846,23 @@
       <c r="F2" t="s">
         <v>5</v>
       </c>
-      <c r="G2" t="n">
-        <v>39.68416</v>
-      </c>
-      <c r="H2" t="n">
+      <c r="G2">
+        <v>39.684159999999999</v>
+      </c>
+      <c r="H2">
         <v>26.97946</v>
       </c>
-      <c r="I2" t="n">
-        <v>40.68416</v>
-      </c>
-      <c r="J2" t="n">
+      <c r="I2">
+        <v>40.684159999999999</v>
+      </c>
+      <c r="J2">
         <v>27.97946</v>
       </c>
-      <c r="K2" t="n">
-        <v>14.0</v>
-      </c>
-      <c r="L2" t="n">
-        <v>15.0</v>
+      <c r="K2">
+        <v>14</v>
+      </c>
+      <c r="L2">
+        <v>15</v>
       </c>
       <c r="M2" t="s">
         <v>6</v>
@@ -539,26 +870,32 @@
       <c r="N2" t="s">
         <v>7</v>
       </c>
-      <c r="O2" t="n">
-        <v>536.0</v>
-      </c>
-      <c r="P2" t="n">
-        <v>10.0</v>
-      </c>
-      <c r="Q2" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="R2" t="n">
-        <v>3.0</v>
+      <c r="O2">
+        <v>536</v>
+      </c>
+      <c r="P2">
+        <v>10</v>
+      </c>
+      <c r="Q2">
+        <v>1</v>
+      </c>
+      <c r="R2">
+        <v>3</v>
       </c>
       <c r="S2" t="s">
         <v>8</v>
       </c>
-      <c r="X2" t="n">
-        <v>1.0</v>
+      <c r="W2" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="X2">
+        <v>1</v>
+      </c>
+      <c r="AR2" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -577,23 +914,23 @@
       <c r="F3" t="s">
         <v>5</v>
       </c>
-      <c r="G3" t="n">
-        <v>39.68416</v>
-      </c>
-      <c r="H3" t="n">
+      <c r="G3">
+        <v>39.684159999999999</v>
+      </c>
+      <c r="H3">
         <v>26.97946</v>
       </c>
-      <c r="I3" t="n">
-        <v>40.68416</v>
-      </c>
-      <c r="J3" t="n">
+      <c r="I3">
+        <v>40.684159999999999</v>
+      </c>
+      <c r="J3">
         <v>27.97946</v>
       </c>
-      <c r="K3" t="n">
-        <v>14.0</v>
-      </c>
-      <c r="L3" t="n">
-        <v>15.0</v>
+      <c r="K3">
+        <v>14</v>
+      </c>
+      <c r="L3">
+        <v>15</v>
       </c>
       <c r="M3" t="s">
         <v>6</v>
@@ -601,26 +938,32 @@
       <c r="N3" t="s">
         <v>7</v>
       </c>
-      <c r="O3" t="n">
-        <v>536.0</v>
-      </c>
-      <c r="P3" t="n">
-        <v>10.0</v>
-      </c>
-      <c r="Q3" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="R3" t="n">
-        <v>10.0</v>
+      <c r="O3">
+        <v>536</v>
+      </c>
+      <c r="P3">
+        <v>10</v>
+      </c>
+      <c r="Q3">
+        <v>3</v>
+      </c>
+      <c r="R3">
+        <v>10</v>
       </c>
       <c r="S3" t="s">
         <v>9</v>
       </c>
-      <c r="X3" t="n">
-        <v>2.0</v>
+      <c r="W3" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="X3">
+        <v>2</v>
+      </c>
+      <c r="AR3" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -639,23 +982,23 @@
       <c r="F4" t="s">
         <v>13</v>
       </c>
-      <c r="G4" t="n">
-        <v>38.68416</v>
-      </c>
-      <c r="H4" t="n">
+      <c r="G4">
+        <v>38.684159999999999</v>
+      </c>
+      <c r="H4">
         <v>25.97946</v>
       </c>
-      <c r="I4" t="n">
-        <v>39.68416</v>
-      </c>
-      <c r="J4" t="n">
+      <c r="I4">
+        <v>39.684159999999999</v>
+      </c>
+      <c r="J4">
         <v>26.97946</v>
       </c>
-      <c r="K4" t="n">
-        <v>14.0</v>
-      </c>
-      <c r="L4" t="n">
-        <v>15.0</v>
+      <c r="K4">
+        <v>14</v>
+      </c>
+      <c r="L4">
+        <v>15</v>
       </c>
       <c r="M4" t="s">
         <v>6</v>
@@ -663,17 +1006,17 @@
       <c r="N4" t="s">
         <v>7</v>
       </c>
-      <c r="O4" t="n">
-        <v>537.0</v>
-      </c>
-      <c r="P4" t="n">
-        <v>10.0</v>
-      </c>
-      <c r="Q4" t="n">
-        <v>11.0</v>
-      </c>
-      <c r="R4" t="n">
-        <v>13.0</v>
+      <c r="O4">
+        <v>537</v>
+      </c>
+      <c r="P4">
+        <v>10</v>
+      </c>
+      <c r="Q4">
+        <v>11</v>
+      </c>
+      <c r="R4">
+        <v>13</v>
       </c>
       <c r="S4" t="s">
         <v>14</v>
@@ -687,13 +1030,13 @@
       <c r="V4" t="s">
         <v>17</v>
       </c>
-      <c r="W4" t="s">
-        <v>18</v>
-      </c>
-      <c r="X4" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="Y4" t="n">
+      <c r="W4" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="X4">
+        <v>1</v>
+      </c>
+      <c r="Y4">
         <v>50.5</v>
       </c>
       <c r="Z4" t="s">
@@ -750,8 +1093,11 @@
       <c r="AQ4" t="s">
         <v>34</v>
       </c>
+      <c r="AR4" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -770,23 +1116,23 @@
       <c r="F5" t="s">
         <v>38</v>
       </c>
-      <c r="G5" t="n">
-        <v>38.7</v>
-      </c>
-      <c r="H5" t="n">
-        <v>26.0</v>
-      </c>
-      <c r="I5" t="n">
-        <v>39.7</v>
-      </c>
-      <c r="J5" t="n">
-        <v>27.0</v>
-      </c>
-      <c r="K5" t="n">
-        <v>15.0</v>
-      </c>
-      <c r="L5" t="n">
-        <v>16.0</v>
+      <c r="G5">
+        <v>38.700000000000003</v>
+      </c>
+      <c r="H5">
+        <v>26</v>
+      </c>
+      <c r="I5">
+        <v>39.700000000000003</v>
+      </c>
+      <c r="J5">
+        <v>27</v>
+      </c>
+      <c r="K5">
+        <v>15</v>
+      </c>
+      <c r="L5">
+        <v>16</v>
       </c>
       <c r="M5" t="s">
         <v>39</v>
@@ -794,17 +1140,17 @@
       <c r="N5" t="s">
         <v>40</v>
       </c>
-      <c r="O5" t="n">
-        <v>566.0</v>
-      </c>
-      <c r="P5" t="n">
-        <v>11.0</v>
-      </c>
-      <c r="Q5" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="R5" t="n">
-        <v>11.0</v>
+      <c r="O5">
+        <v>566</v>
+      </c>
+      <c r="P5">
+        <v>11</v>
+      </c>
+      <c r="Q5">
+        <v>2</v>
+      </c>
+      <c r="R5">
+        <v>11</v>
       </c>
       <c r="S5" t="s">
         <v>41</v>
@@ -818,13 +1164,13 @@
       <c r="V5" t="s">
         <v>30</v>
       </c>
-      <c r="W5" t="s">
-        <v>44</v>
-      </c>
-      <c r="X5" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="Y5" t="n">
+      <c r="W5" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="X5">
+        <v>2</v>
+      </c>
+      <c r="Y5">
         <v>51.5</v>
       </c>
       <c r="Z5" t="s">
@@ -878,8 +1224,11 @@
       <c r="AQ5" t="s">
         <v>25</v>
       </c>
+      <c r="AR5" s="1" t="s">
+        <v>44</v>
+      </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -895,17 +1244,17 @@
       <c r="E6" t="s">
         <v>37</v>
       </c>
-      <c r="G6" t="n">
-        <v>38.7</v>
-      </c>
-      <c r="H6" t="n">
-        <v>26.0</v>
-      </c>
-      <c r="I6" t="n">
-        <v>39.7</v>
-      </c>
-      <c r="J6" t="n">
-        <v>27.0</v>
+      <c r="G6">
+        <v>38.700000000000003</v>
+      </c>
+      <c r="H6">
+        <v>26</v>
+      </c>
+      <c r="I6">
+        <v>39.700000000000003</v>
+      </c>
+      <c r="J6">
+        <v>27</v>
       </c>
       <c r="M6" t="s">
         <v>43</v>
@@ -913,11 +1262,17 @@
       <c r="N6" t="s">
         <v>40</v>
       </c>
-      <c r="X6" t="n">
-        <v>3.0</v>
+      <c r="W6" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="X6">
+        <v>3</v>
+      </c>
+      <c r="AR6" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update export to display multiple geologic ages as a comma delimited list
(cherry picked from commit a0278d68986ee8c4ec9dde7b9888cb604c9d219c)
</commit_message>
<xml_diff>
--- a/geosamples-ingest-service/src/test/resources/test-export.xlsx
+++ b/geosamples-ingest-service/src/test/resources/test-export.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paytoncain/Documents/projects/geology/geosamples-ingest/geosamples-ingest-service/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1783F56D-A326-FD42-8E13-CA65A115B3ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DE20772-8ED7-D440-A038-3D2CE607EA2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-50000" yWindow="500" windowWidth="50000" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1200" yWindow="760" windowWidth="29040" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Output" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="101">
   <si>
     <t>GEOMAR</t>
   </si>
@@ -76,9 +76,6 @@
     <t>7</t>
   </si>
   <si>
-    <t>58</t>
-  </si>
-  <si>
     <t>11</t>
   </si>
   <si>
@@ -154,9 +151,6 @@
     <t>2</t>
   </si>
   <si>
-    <t>54</t>
-  </si>
-  <si>
     <t>09</t>
   </si>
   <si>
@@ -325,7 +319,10 @@
     <t>Other Component Code (6)</t>
   </si>
   <si>
-    <t>00</t>
+    <t>00, 54</t>
+  </si>
+  <si>
+    <t>00, 58</t>
   </si>
 </sst>
 </file>
@@ -687,144 +684,141 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AR6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
+      <selection activeCell="AR6" sqref="AR1:AR6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" t="s">
         <v>58</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>59</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>60</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>61</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>62</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>63</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>64</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>65</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>66</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>67</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>68</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>69</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>70</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>71</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>72</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>73</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>74</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
         <v>75</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
         <v>76</v>
       </c>
-      <c r="T1" t="s">
+      <c r="V1" t="s">
         <v>77</v>
       </c>
-      <c r="U1" t="s">
+      <c r="W1" t="s">
         <v>78</v>
       </c>
-      <c r="V1" t="s">
+      <c r="X1" t="s">
         <v>79</v>
       </c>
-      <c r="W1" t="s">
+      <c r="Y1" t="s">
         <v>80</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Z1" t="s">
         <v>81</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AA1" t="s">
         <v>82</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AB1" t="s">
         <v>83</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AC1" t="s">
         <v>84</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AD1" t="s">
         <v>85</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AE1" t="s">
         <v>86</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AF1" t="s">
         <v>87</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AG1" t="s">
         <v>88</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AH1" t="s">
         <v>89</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AI1" t="s">
         <v>90</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AJ1" t="s">
         <v>91</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AK1" t="s">
         <v>92</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AL1" t="s">
         <v>93</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AM1" t="s">
         <v>94</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AN1" t="s">
         <v>95</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AO1" t="s">
         <v>96</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AP1" t="s">
         <v>97</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AQ1" t="s">
         <v>98</v>
-      </c>
-      <c r="AP1" t="s">
-        <v>99</v>
-      </c>
-      <c r="AQ1" t="s">
-        <v>100</v>
-      </c>
-      <c r="AR1" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:44" x14ac:dyDescent="0.2">
@@ -886,14 +880,12 @@
         <v>8</v>
       </c>
       <c r="W2" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="X2">
         <v>1</v>
       </c>
-      <c r="AR2" s="1" t="s">
-        <v>44</v>
-      </c>
+      <c r="AR2" s="1"/>
     </row>
     <row r="3" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -954,14 +946,12 @@
         <v>9</v>
       </c>
       <c r="W3" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="X3">
         <v>2</v>
       </c>
-      <c r="AR3" s="1" t="s">
-        <v>18</v>
-      </c>
+      <c r="AR3" s="1"/>
     </row>
     <row r="4" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -1031,7 +1021,7 @@
         <v>17</v>
       </c>
       <c r="W4" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="X4">
         <v>1</v>
@@ -1040,62 +1030,60 @@
         <v>50.5</v>
       </c>
       <c r="Z4" t="s">
+        <v>18</v>
+      </c>
+      <c r="AA4" t="s">
         <v>19</v>
       </c>
-      <c r="AA4" t="s">
+      <c r="AB4" t="s">
         <v>20</v>
       </c>
-      <c r="AB4" t="s">
+      <c r="AC4" t="s">
         <v>21</v>
-      </c>
-      <c r="AC4" t="s">
-        <v>22</v>
       </c>
       <c r="AD4" t="s">
         <v>8</v>
       </c>
       <c r="AE4" t="s">
+        <v>22</v>
+      </c>
+      <c r="AF4" t="s">
         <v>23</v>
       </c>
-      <c r="AF4" t="s">
+      <c r="AG4" t="s">
         <v>24</v>
       </c>
-      <c r="AG4" t="s">
+      <c r="AH4" t="s">
         <v>25</v>
       </c>
-      <c r="AH4" t="s">
+      <c r="AI4" t="s">
         <v>26</v>
       </c>
-      <c r="AI4" t="s">
+      <c r="AJ4" t="s">
         <v>27</v>
       </c>
-      <c r="AJ4" t="s">
+      <c r="AK4" t="s">
         <v>28</v>
       </c>
-      <c r="AK4" t="s">
+      <c r="AL4" t="s">
         <v>29</v>
       </c>
-      <c r="AL4" t="s">
+      <c r="AM4" t="s">
         <v>30</v>
-      </c>
-      <c r="AM4" t="s">
-        <v>31</v>
       </c>
       <c r="AN4" t="s">
         <v>15</v>
       </c>
       <c r="AO4" t="s">
+        <v>31</v>
+      </c>
+      <c r="AP4" t="s">
         <v>32</v>
       </c>
-      <c r="AP4" t="s">
+      <c r="AQ4" t="s">
         <v>33</v>
       </c>
-      <c r="AQ4" t="s">
-        <v>34</v>
-      </c>
-      <c r="AR4" s="1" t="s">
-        <v>18</v>
-      </c>
+      <c r="AR4" s="1"/>
     </row>
     <row r="5" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -1105,16 +1093,16 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" t="s">
         <v>35</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>36</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>37</v>
-      </c>
-      <c r="F5" t="s">
-        <v>38</v>
       </c>
       <c r="G5">
         <v>38.700000000000003</v>
@@ -1135,10 +1123,10 @@
         <v>16</v>
       </c>
       <c r="M5" t="s">
+        <v>38</v>
+      </c>
+      <c r="N5" t="s">
         <v>39</v>
-      </c>
-      <c r="N5" t="s">
-        <v>40</v>
       </c>
       <c r="O5">
         <v>566</v>
@@ -1153,19 +1141,19 @@
         <v>11</v>
       </c>
       <c r="S5" t="s">
+        <v>40</v>
+      </c>
+      <c r="T5" t="s">
         <v>41</v>
       </c>
-      <c r="T5" t="s">
+      <c r="U5" t="s">
         <v>42</v>
       </c>
-      <c r="U5" t="s">
-        <v>43</v>
-      </c>
       <c r="V5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="W5" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="X5">
         <v>2</v>
@@ -1174,59 +1162,57 @@
         <v>51.5</v>
       </c>
       <c r="Z5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="AA5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="AB5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AC5" t="s">
         <v>9</v>
       </c>
       <c r="AD5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AE5" t="s">
+        <v>45</v>
+      </c>
+      <c r="AF5" t="s">
+        <v>46</v>
+      </c>
+      <c r="AG5" t="s">
+        <v>24</v>
+      </c>
+      <c r="AI5" t="s">
         <v>47</v>
       </c>
-      <c r="AF5" t="s">
+      <c r="AJ5" t="s">
         <v>48</v>
       </c>
-      <c r="AG5" t="s">
-        <v>25</v>
-      </c>
-      <c r="AI5" t="s">
+      <c r="AK5" t="s">
         <v>49</v>
       </c>
-      <c r="AJ5" t="s">
+      <c r="AL5" t="s">
+        <v>29</v>
+      </c>
+      <c r="AM5" t="s">
         <v>50</v>
       </c>
-      <c r="AK5" t="s">
+      <c r="AN5" t="s">
         <v>51</v>
       </c>
-      <c r="AL5" t="s">
-        <v>30</v>
-      </c>
-      <c r="AM5" t="s">
+      <c r="AO5" t="s">
         <v>52</v>
       </c>
-      <c r="AN5" t="s">
+      <c r="AP5" t="s">
         <v>53</v>
       </c>
-      <c r="AO5" t="s">
-        <v>54</v>
-      </c>
-      <c r="AP5" t="s">
-        <v>55</v>
-      </c>
       <c r="AQ5" t="s">
-        <v>25</v>
-      </c>
-      <c r="AR5" s="1" t="s">
-        <v>44</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="AR5" s="1"/>
     </row>
     <row r="6" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -1236,13 +1222,13 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G6">
         <v>38.700000000000003</v>
@@ -1257,20 +1243,18 @@
         <v>27</v>
       </c>
       <c r="M6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="W6" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="X6">
         <v>3</v>
       </c>
-      <c r="AR6" s="1" t="s">
-        <v>18</v>
-      </c>
+      <c r="AR6" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
IMLGS-223 Sample Comments and Sample Lake add to spreadsheet
</commit_message>
<xml_diff>
--- a/geosamples-ingest-service/src/test/resources/test-export.xlsx
+++ b/geosamples-ingest-service/src/test/resources/test-export.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paytoncain/Documents/projects/geology/geosamples-ingest/geosamples-ingest-service/src/test/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peemin/Projects/IMLGS_geosamples-ingest/geosamples-ingest/geosamples-ingest-service/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DE20772-8ED7-D440-A038-3D2CE607EA2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16CB8D38-3CB7-ED42-B8AC-F139263BEDEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1200" yWindow="760" windowWidth="29040" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19540" yWindow="24260" windowWidth="32520" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Output" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="111">
   <si>
     <t>GEOMAR</t>
   </si>
@@ -323,6 +323,36 @@
   </si>
   <si>
     <t>00, 58</t>
+  </si>
+  <si>
+    <t>Lake</t>
+  </si>
+  <si>
+    <t>Lake 4</t>
+  </si>
+  <si>
+    <t>Lake 1</t>
+  </si>
+  <si>
+    <t>Lake 2</t>
+  </si>
+  <si>
+    <t>Lake 3</t>
+  </si>
+  <si>
+    <t>Sample Comments</t>
+  </si>
+  <si>
+    <t>Sample comment 4</t>
+  </si>
+  <si>
+    <t>Sample comment 3</t>
+  </si>
+  <si>
+    <t>Sample comment 2</t>
+  </si>
+  <si>
+    <t>Sample comment 1</t>
   </si>
 </sst>
 </file>
@@ -682,15 +712,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AR6"/>
+  <dimension ref="A1:AS6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
-      <selection activeCell="AR6" sqref="AR1:AR6"/>
+    <sheetView tabSelected="1" topLeftCell="AF1" workbookViewId="0">
+      <selection activeCell="AS5" sqref="AS5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="19.5" customWidth="1"/>
+    <col min="45" max="45" width="15.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>56</v>
       </c>
@@ -820,8 +854,14 @@
       <c r="AQ1" t="s">
         <v>98</v>
       </c>
+      <c r="AR1" t="s">
+        <v>101</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>106</v>
+      </c>
     </row>
-    <row r="2" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -885,9 +925,14 @@
       <c r="X2">
         <v>1</v>
       </c>
-      <c r="AR2" s="1"/>
+      <c r="AR2" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="AS2" s="1" t="s">
+        <v>107</v>
+      </c>
     </row>
-    <row r="3" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -951,9 +996,14 @@
       <c r="X3">
         <v>2</v>
       </c>
-      <c r="AR3" s="1"/>
+      <c r="AR3" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="AS3" s="1" t="s">
+        <v>107</v>
+      </c>
     </row>
-    <row r="4" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -1083,9 +1133,14 @@
       <c r="AQ4" t="s">
         <v>33</v>
       </c>
-      <c r="AR4" s="1"/>
+      <c r="AR4" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="AS4" s="1" t="s">
+        <v>110</v>
+      </c>
     </row>
-    <row r="5" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -1212,9 +1267,14 @@
       <c r="AQ5" t="s">
         <v>24</v>
       </c>
-      <c r="AR5" s="1"/>
+      <c r="AR5" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="AS5" s="1" t="s">
+        <v>109</v>
+      </c>
     </row>
-    <row r="6" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -1254,7 +1314,12 @@
       <c r="X6">
         <v>3</v>
       </c>
-      <c r="AR6" s="1"/>
+      <c r="AR6" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="AS6" s="1" t="s">
+        <v>108</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
IMLGS-223 child interval spreadsheet
</commit_message>
<xml_diff>
--- a/geosamples-ingest-service/src/test/resources/test-export.xlsx
+++ b/geosamples-ingest-service/src/test/resources/test-export.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peemin/Projects/IMLGS_geosamples-ingest/geosamples-ingest/geosamples-ingest-service/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16CB8D38-3CB7-ED42-B8AC-F139263BEDEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3787BDFD-B090-6B4E-87A8-8502AF1993A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19540" yWindow="24260" windowWidth="32520" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-34600" yWindow="6960" windowWidth="32520" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Output" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="115">
   <si>
     <t>GEOMAR</t>
   </si>
@@ -259,100 +259,112 @@
     <t>Geologic Age Code</t>
   </si>
   <si>
+    <t>Bulk Weight</t>
+  </si>
+  <si>
+    <t>Physiographic Province Code</t>
+  </si>
+  <si>
+    <t>Sample Lithology Code</t>
+  </si>
+  <si>
+    <t>Sample Mineralogy Code</t>
+  </si>
+  <si>
+    <t>Sample Weathering or Metamorphism Code</t>
+  </si>
+  <si>
+    <t>Glass Remarks Code</t>
+  </si>
+  <si>
+    <t>Munsell Color</t>
+  </si>
+  <si>
+    <t>Principal Investigator</t>
+  </si>
+  <si>
+    <t>Sample Not Available</t>
+  </si>
+  <si>
+    <t>IGSN</t>
+  </si>
+  <si>
+    <t>Alternate Leg</t>
+  </si>
+  <si>
+    <t>Free form Description of Composition</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Other Component Code (1)</t>
+  </si>
+  <si>
+    <t>Other Component Code (2)</t>
+  </si>
+  <si>
+    <t>Other Component Code (3)</t>
+  </si>
+  <si>
+    <t>Other Component Code (4)</t>
+  </si>
+  <si>
+    <t>Other Component Code (5)</t>
+  </si>
+  <si>
+    <t>Other Component Code (6)</t>
+  </si>
+  <si>
+    <t>00, 54</t>
+  </si>
+  <si>
+    <t>00, 58</t>
+  </si>
+  <si>
+    <t>Lake</t>
+  </si>
+  <si>
+    <t>Lake 4</t>
+  </si>
+  <si>
+    <t>Lake 1</t>
+  </si>
+  <si>
+    <t>Lake 2</t>
+  </si>
+  <si>
+    <t>Lake 3</t>
+  </si>
+  <si>
+    <t>Sample Comments</t>
+  </si>
+  <si>
+    <t>Sample comment 4</t>
+  </si>
+  <si>
+    <t>Sample comment 3</t>
+  </si>
+  <si>
+    <t>Sample comment 2</t>
+  </si>
+  <si>
+    <t>Sample comment 1</t>
+  </si>
+  <si>
     <t>Interval</t>
   </si>
   <si>
-    <t>Bulk Weight</t>
-  </si>
-  <si>
-    <t>Physiographic Province Code</t>
-  </si>
-  <si>
-    <t>Sample Lithology Code</t>
-  </si>
-  <si>
-    <t>Sample Mineralogy Code</t>
-  </si>
-  <si>
-    <t>Sample Weathering or Metamorphism Code</t>
-  </si>
-  <si>
-    <t>Glass Remarks Code</t>
-  </si>
-  <si>
-    <t>Munsell Color</t>
-  </si>
-  <si>
-    <t>Principal Investigator</t>
-  </si>
-  <si>
-    <t>Sample Not Available</t>
-  </si>
-  <si>
-    <t>IGSN</t>
-  </si>
-  <si>
-    <t>Alternate Leg</t>
-  </si>
-  <si>
-    <t>Free form Description of Composition</t>
-  </si>
-  <si>
-    <t>Comments</t>
-  </si>
-  <si>
-    <t>Other Component Code (1)</t>
-  </si>
-  <si>
-    <t>Other Component Code (2)</t>
-  </si>
-  <si>
-    <t>Other Component Code (3)</t>
-  </si>
-  <si>
-    <t>Other Component Code (4)</t>
-  </si>
-  <si>
-    <t>Other Component Code (5)</t>
-  </si>
-  <si>
-    <t>Other Component Code (6)</t>
-  </si>
-  <si>
-    <t>00, 54</t>
-  </si>
-  <si>
-    <t>00, 58</t>
-  </si>
-  <si>
-    <t>Lake</t>
-  </si>
-  <si>
-    <t>Lake 4</t>
-  </si>
-  <si>
-    <t>Lake 1</t>
-  </si>
-  <si>
-    <t>Lake 2</t>
-  </si>
-  <si>
-    <t>Lake 3</t>
-  </si>
-  <si>
-    <t>Sample Comments</t>
-  </si>
-  <si>
-    <t>Sample comment 4</t>
-  </si>
-  <si>
-    <t>Sample comment 3</t>
-  </si>
-  <si>
-    <t>Sample comment 2</t>
-  </si>
-  <si>
-    <t>Sample comment 1</t>
+    <t>Interval/Subsample IGSN</t>
+  </si>
+  <si>
+    <t>child1</t>
+  </si>
+  <si>
+    <t>child2</t>
+  </si>
+  <si>
+    <t>child3</t>
   </si>
 </sst>
 </file>
@@ -712,19 +724,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AS6"/>
+  <dimension ref="A1:AT6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AF1" workbookViewId="0">
-      <selection activeCell="AS5" sqref="AS5"/>
+    <sheetView tabSelected="1" topLeftCell="AG1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="AH1" sqref="AH1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="19.5" customWidth="1"/>
+    <col min="33" max="33" width="20.1640625" customWidth="1"/>
+    <col min="35" max="35" width="19.5" customWidth="1"/>
+    <col min="36" max="36" width="25.33203125" customWidth="1"/>
+    <col min="37" max="37" width="18" customWidth="1"/>
+    <col min="43" max="43" width="27" customWidth="1"/>
     <col min="45" max="45" width="15.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>56</v>
       </c>
@@ -795,73 +812,76 @@
         <v>78</v>
       </c>
       <c r="X1" t="s">
+        <v>110</v>
+      </c>
+      <c r="Y1" t="s">
         <v>79</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>80</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>81</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>82</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>83</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>84</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>85</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>86</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>87</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>88</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>89</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>90</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>91</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" t="s">
         <v>92</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AM1" t="s">
         <v>93</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AN1" t="s">
         <v>94</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AO1" t="s">
         <v>95</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AP1" t="s">
         <v>96</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AQ1" t="s">
         <v>97</v>
       </c>
-      <c r="AQ1" t="s">
-        <v>98</v>
-      </c>
       <c r="AR1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AS1" t="s">
-        <v>106</v>
+        <v>105</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>111</v>
       </c>
     </row>
-    <row r="2" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -920,19 +940,19 @@
         <v>8</v>
       </c>
       <c r="W2" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="X2">
         <v>1</v>
       </c>
       <c r="AR2" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AS2" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
-    <row r="3" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -991,19 +1011,19 @@
         <v>9</v>
       </c>
       <c r="W3" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="X3">
         <v>2</v>
       </c>
       <c r="AR3" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AS3" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
-    <row r="4" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -1071,7 +1091,7 @@
         <v>17</v>
       </c>
       <c r="W4" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="X4">
         <v>1</v>
@@ -1134,13 +1154,16 @@
         <v>33</v>
       </c>
       <c r="AR4" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AS4" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
+      </c>
+      <c r="AT4" t="s">
+        <v>112</v>
       </c>
     </row>
-    <row r="5" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -1208,7 +1231,7 @@
         <v>29</v>
       </c>
       <c r="W5" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="X5">
         <v>2</v>
@@ -1268,13 +1291,16 @@
         <v>24</v>
       </c>
       <c r="AR5" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="AS5" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
+      </c>
+      <c r="AT5" t="s">
+        <v>113</v>
       </c>
     </row>
-    <row r="6" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -1309,16 +1335,19 @@
         <v>39</v>
       </c>
       <c r="W6" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="X6">
         <v>3</v>
       </c>
       <c r="AR6" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AS6" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
+      </c>
+      <c r="AT6" t="s">
+        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>